<commit_message>
before adoption of enclosure model in HR
</commit_message>
<xml_diff>
--- a/00_nightly_only/dev/ABSSelfExplore/test.xlsx
+++ b/00_nightly_only/dev/ABSSelfExplore/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RBI\Documents\tidycells_nightly\00_nightly_only\dev\ABSSelfExplore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A67DC08-6C2E-4B7D-87CC-EBF719D4DB50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BC7EE6-ED8E-4572-B1BC-178E74F72F8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{885F78D0-ECCA-4EBD-90DB-2579D593F982}">
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{885F78D0-ECCA-4EBD-90DB-2579D593F982}">
       <text>
         <r>
           <rPr>
@@ -58,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{FBB4FA3D-B749-4250-A4E8-311EC73BB95B}">
+    <comment ref="J6" authorId="0" shapeId="0" xr:uid="{FBB4FA3D-B749-4250-A4E8-311EC73BB95B}">
       <text>
         <r>
           <rPr>
@@ -70,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J6" authorId="0" shapeId="0" xr:uid="{BB1D119E-D8DA-439F-8908-2E2A6602B4EE}">
+    <comment ref="K6" authorId="0" shapeId="0" xr:uid="{BB1D119E-D8DA-439F-8908-2E2A6602B4EE}">
       <text>
         <r>
           <rPr>
@@ -82,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M6" authorId="0" shapeId="0" xr:uid="{3CC94AFA-A78C-4ED7-BC49-A8C68857D104}">
+    <comment ref="N6" authorId="0" shapeId="0" xr:uid="{3CC94AFA-A78C-4ED7-BC49-A8C68857D104}">
       <text>
         <r>
           <rPr>
@@ -94,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q6" authorId="0" shapeId="0" xr:uid="{407E78B2-188D-41E1-9691-4076EA70F102}">
+    <comment ref="R6" authorId="0" shapeId="0" xr:uid="{407E78B2-188D-41E1-9691-4076EA70F102}">
       <text>
         <r>
           <rPr>
@@ -143,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{181947EE-D706-4960-AAE1-C7FB159F517E}">
+    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{181947EE-D706-4960-AAE1-C7FB159F517E}">
       <text>
         <r>
           <rPr>
@@ -179,319 +179,319 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{E735D3AB-18F5-4654-B735-2E2CCA5AA7D4}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{CCFD9025-40DE-4C6E-A9BC-B9790E8A2EC6}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E17" authorId="0" shapeId="0" xr:uid="{AB509105-AA5B-4B29-A8C3-6FC1C4994D4B}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C18" authorId="0" shapeId="0" xr:uid="{F784A78B-7DC4-4590-B82D-1687E9C2AF9E}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{E789A6CD-4F4A-41FA-BFC7-34780F0AB2CC}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{D2BF655E-DCF9-4F7B-A34D-CDEA696C03E1}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{3864503C-6F43-42C6-AF4D-28B611BBE58A}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{5198022E-C94E-4450-86C0-15C7BE88F43D}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E19" authorId="0" shapeId="0" xr:uid="{7A33FF57-F625-4C6D-B6EB-9FB208B4CED4}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{A6CFC32E-B67C-4144-9C21-4983AA4D2B49}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{4175EFB0-8E42-4AE7-879C-94E8E67600DE}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{C8A58C6F-62D9-40B4-ADAE-1B3BB167D2A0}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C21" authorId="0" shapeId="0" xr:uid="{9C1300CF-854A-47F2-85F2-1A4E5508CAD1}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{DD05E0D3-BE9A-4504-9363-72AA4EC24A09}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E21" authorId="0" shapeId="0" xr:uid="{606EE025-6503-4638-92BD-FC58D4D3C79C}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{41DF1E39-F569-4399-BA63-7E292C2B898F}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{BC424FC8-2796-4F71-93CC-E0DEB19F0E9E}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{F9C9B750-F137-47AF-B2CB-6DD34BE67EF4}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C23" authorId="0" shapeId="0" xr:uid="{C010E479-8083-4792-A2FE-1994C9DDFC82}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{7C9E27E2-DC73-42A1-9948-6A900756411C}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E23" authorId="0" shapeId="0" xr:uid="{48B4FAFC-F896-4F29-8B65-888F68D78336}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C24" authorId="0" shapeId="0" xr:uid="{732BF5F1-FCC3-42ED-A5A7-7E04EF94CC3C}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D24" authorId="0" shapeId="0" xr:uid="{490C0F2E-CBC8-4E55-A1E8-1457E220B79A}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E24" authorId="0" shapeId="0" xr:uid="{C483ED4E-78E1-4986-A453-3FDC4F2B9648}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C25" authorId="0" shapeId="0" xr:uid="{03B27C89-75F8-4F5A-A934-0F4311C7D8B8}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D25" authorId="0" shapeId="0" xr:uid="{9893BB1C-1682-4B34-A74B-122B3F2BC1D6}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E25" authorId="0" shapeId="0" xr:uid="{1B721C68-6F94-4CA4-A5F1-205A02D4B6ED}">
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{E735D3AB-18F5-4654-B735-2E2CCA5AA7D4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E17" authorId="0" shapeId="0" xr:uid="{CCFD9025-40DE-4C6E-A9BC-B9790E8A2EC6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{AB509105-AA5B-4B29-A8C3-6FC1C4994D4B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{F784A78B-7DC4-4590-B82D-1687E9C2AF9E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{E789A6CD-4F4A-41FA-BFC7-34780F0AB2CC}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{D2BF655E-DCF9-4F7B-A34D-CDEA696C03E1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{3864503C-6F43-42C6-AF4D-28B611BBE58A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E19" authorId="0" shapeId="0" xr:uid="{5198022E-C94E-4450-86C0-15C7BE88F43D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{7A33FF57-F625-4C6D-B6EB-9FB208B4CED4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{A6CFC32E-B67C-4144-9C21-4983AA4D2B49}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{4175EFB0-8E42-4AE7-879C-94E8E67600DE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{C8A58C6F-62D9-40B4-ADAE-1B3BB167D2A0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{9C1300CF-854A-47F2-85F2-1A4E5508CAD1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E21" authorId="0" shapeId="0" xr:uid="{DD05E0D3-BE9A-4504-9363-72AA4EC24A09}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F21" authorId="0" shapeId="0" xr:uid="{606EE025-6503-4638-92BD-FC58D4D3C79C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{41DF1E39-F569-4399-BA63-7E292C2B898F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{BC424FC8-2796-4F71-93CC-E0DEB19F0E9E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{F9C9B750-F137-47AF-B2CB-6DD34BE67EF4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{C010E479-8083-4792-A2FE-1994C9DDFC82}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E23" authorId="0" shapeId="0" xr:uid="{7C9E27E2-DC73-42A1-9948-6A900756411C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{48B4FAFC-F896-4F29-8B65-888F68D78336}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D24" authorId="0" shapeId="0" xr:uid="{732BF5F1-FCC3-42ED-A5A7-7E04EF94CC3C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E24" authorId="0" shapeId="0" xr:uid="{490C0F2E-CBC8-4E55-A1E8-1457E220B79A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{C483ED4E-78E1-4986-A453-3FDC4F2B9648}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D25" authorId="0" shapeId="0" xr:uid="{03B27C89-75F8-4F5A-A934-0F4311C7D8B8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E25" authorId="0" shapeId="0" xr:uid="{9893BB1C-1682-4B34-A74B-122B3F2BC1D6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{1B721C68-6F94-4CA4-A5F1-205A02D4B6ED}">
       <text>
         <r>
           <rPr>
@@ -515,67 +515,67 @@
         </r>
       </text>
     </comment>
-    <comment ref="C27" authorId="0" shapeId="0" xr:uid="{DEBBDCA8-8273-420A-AEE9-92485CA1052F}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D27" authorId="0" shapeId="0" xr:uid="{3AF55651-DEED-4DD9-9610-E18125566EB3}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E27" authorId="0" shapeId="0" xr:uid="{3F837F52-00B3-452C-9AEE-4C74A6DFDA27}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C28" authorId="0" shapeId="0" xr:uid="{5CEE936D-471D-4604-9393-501387D79CDB}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{B7FB4A8D-A475-4782-8ED7-08E6D42C3356}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E28" authorId="0" shapeId="0" xr:uid="{399D3620-3265-4344-A440-912DD0F8252B}">
+    <comment ref="D27" authorId="0" shapeId="0" xr:uid="{DEBBDCA8-8273-420A-AEE9-92485CA1052F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E27" authorId="0" shapeId="0" xr:uid="{3AF55651-DEED-4DD9-9610-E18125566EB3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{3F837F52-00B3-452C-9AEE-4C74A6DFDA27}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{5CEE936D-471D-4604-9393-501387D79CDB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E28" authorId="0" shapeId="0" xr:uid="{B7FB4A8D-A475-4782-8ED7-08E6D42C3356}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{399D3620-3265-4344-A440-912DD0F8252B}">
       <text>
         <r>
           <rPr>
@@ -599,67 +599,67 @@
         </r>
       </text>
     </comment>
-    <comment ref="C30" authorId="0" shapeId="0" xr:uid="{A4C0A529-925D-4C9F-A26A-EA736C4AA1DE}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D30" authorId="0" shapeId="0" xr:uid="{A89FF431-A93A-43FA-B57E-1D3DCA3B14E8}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E30" authorId="0" shapeId="0" xr:uid="{AD0571CD-A56A-4B9E-90F0-B7FF8E87C3DE}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C31" authorId="0" shapeId="0" xr:uid="{2EC8D018-FE8D-47D6-8514-502C8BD94ED8}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D31" authorId="0" shapeId="0" xr:uid="{40BBD6E3-42CB-4FE8-BA28-560C96EEE4FE}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E31" authorId="0" shapeId="0" xr:uid="{DF1F722F-9164-4A2A-8F47-62D59A3DAA22}">
+    <comment ref="D30" authorId="0" shapeId="0" xr:uid="{A4C0A529-925D-4C9F-A26A-EA736C4AA1DE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E30" authorId="0" shapeId="0" xr:uid="{A89FF431-A93A-43FA-B57E-1D3DCA3B14E8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{AD0571CD-A56A-4B9E-90F0-B7FF8E87C3DE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D31" authorId="0" shapeId="0" xr:uid="{2EC8D018-FE8D-47D6-8514-502C8BD94ED8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E31" authorId="0" shapeId="0" xr:uid="{40BBD6E3-42CB-4FE8-BA28-560C96EEE4FE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{DF1F722F-9164-4A2A-8F47-62D59A3DAA22}">
       <text>
         <r>
           <rPr>
@@ -696,103 +696,103 @@
         </r>
       </text>
     </comment>
-    <comment ref="C33" authorId="0" shapeId="0" xr:uid="{A930BEA3-7B40-4E30-A9FD-68B7257922D0}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D33" authorId="0" shapeId="0" xr:uid="{90DF1AE6-E633-4503-8563-25C38093D4ED}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E33" authorId="0" shapeId="0" xr:uid="{9014AB0B-D7A2-4305-A79F-1BFAFBB9B949}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C34" authorId="0" shapeId="0" xr:uid="{DD9C5902-D28A-498B-8CCF-9813B3399C74}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D34" authorId="0" shapeId="0" xr:uid="{C2C3806F-1315-4B05-AE4A-50C623CA9129}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E34" authorId="0" shapeId="0" xr:uid="{CCA370A9-B4F2-4B9A-AB34-2C82F1C2EFBC}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C35" authorId="0" shapeId="0" xr:uid="{26F1CB8A-CC35-430F-88E9-705FC24A5EC6}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D35" authorId="0" shapeId="0" xr:uid="{F99133A7-7573-4B1B-AFDE-7894D9CABD7B}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>not available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E35" authorId="0" shapeId="0" xr:uid="{80102284-3F01-406C-B46B-820DBD41F9A6}">
+    <comment ref="D33" authorId="0" shapeId="0" xr:uid="{A930BEA3-7B40-4E30-A9FD-68B7257922D0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E33" authorId="0" shapeId="0" xr:uid="{90DF1AE6-E633-4503-8563-25C38093D4ED}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{9014AB0B-D7A2-4305-A79F-1BFAFBB9B949}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D34" authorId="0" shapeId="0" xr:uid="{DD9C5902-D28A-498B-8CCF-9813B3399C74}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E34" authorId="0" shapeId="0" xr:uid="{C2C3806F-1315-4B05-AE4A-50C623CA9129}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{CCA370A9-B4F2-4B9A-AB34-2C82F1C2EFBC}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D35" authorId="0" shapeId="0" xr:uid="{26F1CB8A-CC35-430F-88E9-705FC24A5EC6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E35" authorId="0" shapeId="0" xr:uid="{F99133A7-7573-4B1B-AFDE-7894D9CABD7B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>not available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{80102284-3F01-406C-B46B-820DBD41F9A6}">
       <text>
         <r>
           <rPr>
@@ -822,7 +822,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
   <si>
     <t xml:space="preserve">            Australian Bureau of Statistics</t>
   </si>
@@ -972,6 +972,12 @@
   </si>
   <si>
     <t>2016 -&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year  goes here -&gt; </t>
+  </si>
+  <si>
+    <t>Cool Data</t>
   </si>
 </sst>
 </file>
@@ -1130,17 +1136,17 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1423,1386 +1429,1435 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q45"/>
+  <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.75" customWidth="1"/>
+    <col min="1" max="2" width="19.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="36" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:18" ht="36" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+    </row>
+    <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="5"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="5"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="5"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
-    </row>
-    <row r="6" spans="1:17" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="23" t="s">
+      <c r="C5" s="4"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="5"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="5"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="5"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+    </row>
+    <row r="6" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="G6" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="J6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="K6" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="L6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="M6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="N6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="23" t="s">
+      <c r="O6" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="O6" s="6" t="s">
+      <c r="P6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="6" t="s">
+      <c r="Q6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" s="6" t="s">
+      <c r="R6" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="7"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="8"/>
-      <c r="C9" s="9">
+      <c r="C9" s="8"/>
+      <c r="D9" s="9">
         <v>8946</v>
       </c>
-      <c r="D9" s="10">
+      <c r="E9" s="10">
         <v>9</v>
       </c>
-      <c r="E9" s="11">
+      <c r="F9" s="11">
         <v>4.8</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="9"/>
+      <c r="G9" s="11"/>
       <c r="H9" s="9"/>
-      <c r="I9" s="11"/>
+      <c r="I9" s="9"/>
       <c r="J9" s="11"/>
-      <c r="K9" s="9">
+      <c r="K9" s="11"/>
+      <c r="L9" s="9">
         <v>6810</v>
       </c>
-      <c r="L9" s="9">
+      <c r="M9" s="9">
         <v>7</v>
       </c>
-      <c r="M9" s="11">
+      <c r="N9" s="11">
         <v>3.2</v>
       </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="9">
+      <c r="O9" s="11"/>
+      <c r="P9" s="9">
         <v>8200</v>
       </c>
-      <c r="P9" s="9">
+      <c r="Q9" s="9">
         <v>7</v>
       </c>
-      <c r="Q9" s="11">
+      <c r="R9" s="11">
         <v>3.5</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="9">
+      <c r="C10" s="8"/>
+      <c r="D10" s="9">
         <v>13420</v>
       </c>
-      <c r="D10" s="10">
+      <c r="E10" s="10">
         <v>14</v>
       </c>
-      <c r="E10" s="11">
+      <c r="F10" s="11">
         <v>7.2</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="9"/>
+      <c r="G10" s="11"/>
       <c r="H10" s="9"/>
-      <c r="I10" s="11"/>
+      <c r="I10" s="9"/>
       <c r="J10" s="11"/>
-      <c r="K10" s="9">
+      <c r="K10" s="11"/>
+      <c r="L10" s="9">
         <v>21258</v>
       </c>
-      <c r="L10" s="9">
+      <c r="M10" s="9">
         <v>21</v>
       </c>
-      <c r="M10" s="11">
+      <c r="N10" s="11">
         <v>9.9</v>
       </c>
-      <c r="N10" s="11"/>
-      <c r="O10" s="9">
+      <c r="O10" s="11"/>
+      <c r="P10" s="9">
         <v>21235</v>
       </c>
-      <c r="P10" s="9">
+      <c r="Q10" s="9">
         <v>18</v>
       </c>
-      <c r="Q10" s="11">
+      <c r="R10" s="11">
         <v>9.1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="8"/>
-      <c r="C11" s="9">
+      <c r="C11" s="8"/>
+      <c r="D11" s="9">
         <v>17880</v>
       </c>
-      <c r="D11" s="10">
+      <c r="E11" s="10">
         <v>19</v>
       </c>
-      <c r="E11" s="11">
+      <c r="F11" s="11">
         <v>9.5</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="9"/>
+      <c r="G11" s="11"/>
       <c r="H11" s="9"/>
-      <c r="I11" s="11"/>
+      <c r="I11" s="9"/>
       <c r="J11" s="11"/>
-      <c r="K11" s="9"/>
+      <c r="K11" s="11"/>
       <c r="L11" s="9"/>
-      <c r="M11" s="11"/>
+      <c r="M11" s="9"/>
       <c r="N11" s="11"/>
-      <c r="O11" s="9">
+      <c r="O11" s="11"/>
+      <c r="P11" s="9">
         <v>17725</v>
       </c>
-      <c r="P11" s="9">
+      <c r="Q11" s="9">
         <v>15</v>
       </c>
-      <c r="Q11" s="11">
+      <c r="R11" s="11">
         <v>7.6</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="8"/>
-      <c r="C12" s="9">
+      <c r="C12" s="8"/>
+      <c r="D12" s="9">
         <v>21300</v>
       </c>
-      <c r="D12" s="10">
+      <c r="E12" s="10">
         <v>22</v>
       </c>
-      <c r="E12" s="11">
+      <c r="F12" s="11">
         <v>11.4</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="9"/>
+      <c r="G12" s="11"/>
       <c r="H12" s="9"/>
-      <c r="I12" s="11"/>
+      <c r="I12" s="9"/>
       <c r="J12" s="11"/>
-      <c r="K12" s="9"/>
+      <c r="K12" s="11"/>
       <c r="L12" s="9"/>
-      <c r="M12" s="11"/>
+      <c r="M12" s="9"/>
       <c r="N12" s="11"/>
-      <c r="O12" s="9">
+      <c r="O12" s="11"/>
+      <c r="P12" s="9">
         <v>17503</v>
       </c>
-      <c r="P12" s="9">
+      <c r="Q12" s="9">
         <v>15</v>
       </c>
-      <c r="Q12" s="11">
+      <c r="R12" s="11">
         <v>7.5</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8"/>
-      <c r="C13" s="9">
+      <c r="C13" s="8"/>
+      <c r="D13" s="9">
         <v>338</v>
       </c>
-      <c r="D13" s="10">
+      <c r="E13" s="10">
         <v>0</v>
       </c>
-      <c r="E13" s="11">
+      <c r="F13" s="11">
         <v>0.2</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="9">
+      <c r="G13" s="11"/>
+      <c r="H13" s="9">
         <v>500</v>
       </c>
-      <c r="H13" s="9">
+      <c r="I13" s="9">
         <v>1</v>
       </c>
-      <c r="I13" s="11">
+      <c r="J13" s="11">
         <v>0.30000000000000004</v>
       </c>
-      <c r="J13" s="11"/>
-      <c r="K13" s="9"/>
+      <c r="K13" s="11"/>
       <c r="L13" s="9"/>
-      <c r="M13" s="11"/>
+      <c r="M13" s="9"/>
       <c r="N13" s="11"/>
-      <c r="O13" s="9">
+      <c r="O13" s="11"/>
+      <c r="P13" s="9">
         <v>678</v>
       </c>
-      <c r="P13" s="9">
+      <c r="Q13" s="9">
         <v>1</v>
       </c>
-      <c r="Q13" s="11">
+      <c r="R13" s="11">
         <v>0.3</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="8"/>
-      <c r="C14" s="9">
+      <c r="C14" s="8"/>
+      <c r="D14" s="9">
         <v>33430</v>
       </c>
-      <c r="D14" s="10">
+      <c r="E14" s="10">
         <v>35</v>
       </c>
-      <c r="E14" s="11">
+      <c r="F14" s="11">
         <v>17.8</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="9">
+      <c r="G14" s="11"/>
+      <c r="H14" s="9">
         <v>31531</v>
       </c>
-      <c r="H14" s="9">
+      <c r="I14" s="9">
         <v>35</v>
       </c>
-      <c r="I14" s="11">
+      <c r="J14" s="11">
         <v>15.9</v>
       </c>
-      <c r="J14" s="11"/>
-      <c r="K14" s="9"/>
+      <c r="K14" s="11"/>
       <c r="L14" s="9"/>
-      <c r="M14" s="11"/>
+      <c r="M14" s="9"/>
       <c r="N14" s="11"/>
-      <c r="O14" s="9">
+      <c r="O14" s="11"/>
+      <c r="P14" s="9">
         <v>51088</v>
       </c>
-      <c r="P14" s="9">
+      <c r="Q14" s="9">
         <v>44</v>
       </c>
-      <c r="Q14" s="11">
+      <c r="R14" s="11">
         <v>21.8</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="12"/>
-      <c r="C15" s="13">
+      <c r="C15" s="12"/>
+      <c r="D15" s="13">
         <v>95314</v>
       </c>
-      <c r="D15" s="14">
+      <c r="E15" s="14">
         <v>100</v>
       </c>
-      <c r="E15" s="15">
+      <c r="F15" s="15">
         <v>50.8</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="13">
+      <c r="G15" s="15"/>
+      <c r="H15" s="13">
         <v>89728</v>
       </c>
-      <c r="H15" s="13">
+      <c r="I15" s="13">
         <v>100</v>
       </c>
-      <c r="I15" s="15">
+      <c r="J15" s="15">
         <v>45.2</v>
       </c>
-      <c r="J15" s="15"/>
-      <c r="K15" s="13"/>
+      <c r="K15" s="15"/>
       <c r="L15" s="13"/>
-      <c r="M15" s="15"/>
+      <c r="M15" s="13"/>
       <c r="N15" s="15"/>
-      <c r="O15" s="13">
+      <c r="O15" s="15"/>
+      <c r="P15" s="13">
         <v>116427</v>
       </c>
-      <c r="P15" s="13">
+      <c r="Q15" s="13">
         <v>100</v>
       </c>
-      <c r="Q15" s="15">
+      <c r="R15" s="15">
         <v>49.8</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="7"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
       <c r="F17" s="11"/>
-      <c r="G17" s="9">
+      <c r="G17" s="11"/>
+      <c r="H17" s="9">
         <v>15715</v>
       </c>
-      <c r="H17" s="9">
+      <c r="I17" s="9">
         <v>18</v>
       </c>
-      <c r="I17" s="11">
+      <c r="J17" s="11">
         <v>50.5</v>
       </c>
-      <c r="J17" s="11"/>
-      <c r="K17" s="9">
+      <c r="K17" s="11"/>
+      <c r="L17" s="9">
         <v>17767</v>
       </c>
-      <c r="L17" s="9">
+      <c r="M17" s="9">
         <v>17</v>
       </c>
-      <c r="M17" s="11">
+      <c r="N17" s="11">
         <v>53.6</v>
       </c>
-      <c r="N17" s="11"/>
-      <c r="O17" s="9"/>
+      <c r="O17" s="11"/>
       <c r="P17" s="9"/>
-      <c r="Q17" s="11"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q17" s="9"/>
+      <c r="R17" s="11"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="11"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
       <c r="F18" s="11"/>
-      <c r="G18" s="9">
+      <c r="G18" s="11"/>
+      <c r="H18" s="9">
         <v>9788</v>
       </c>
-      <c r="H18" s="9">
+      <c r="I18" s="9">
         <v>11</v>
       </c>
-      <c r="I18" s="11">
+      <c r="J18" s="11">
         <v>51.1</v>
       </c>
-      <c r="J18" s="11"/>
-      <c r="K18" s="9">
+      <c r="K18" s="11"/>
+      <c r="L18" s="9">
         <v>10718</v>
       </c>
-      <c r="L18" s="9">
+      <c r="M18" s="9">
         <v>10</v>
       </c>
-      <c r="M18" s="11">
+      <c r="N18" s="11">
         <v>54.9</v>
       </c>
-      <c r="N18" s="11"/>
-      <c r="O18" s="9"/>
+      <c r="O18" s="11"/>
       <c r="P18" s="9"/>
-      <c r="Q18" s="11"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q18" s="9"/>
+      <c r="R18" s="11"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
       <c r="F19" s="11"/>
-      <c r="G19" s="9">
+      <c r="G19" s="11"/>
+      <c r="H19" s="9">
         <v>12155</v>
       </c>
-      <c r="H19" s="9">
+      <c r="I19" s="9">
         <v>14</v>
       </c>
-      <c r="I19" s="11">
+      <c r="J19" s="11">
         <v>75.400000000000006</v>
       </c>
-      <c r="J19" s="11"/>
-      <c r="K19" s="9">
+      <c r="K19" s="11"/>
+      <c r="L19" s="9">
         <v>14479</v>
       </c>
-      <c r="L19" s="9">
+      <c r="M19" s="9">
         <v>14</v>
       </c>
-      <c r="M19" s="11">
+      <c r="N19" s="11">
         <v>83.1</v>
       </c>
-      <c r="N19" s="11"/>
-      <c r="O19" s="9"/>
+      <c r="O19" s="11"/>
       <c r="P19" s="9"/>
-      <c r="Q19" s="11"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q19" s="9"/>
+      <c r="R19" s="11"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
       <c r="F20" s="11"/>
-      <c r="G20" s="9">
+      <c r="G20" s="11"/>
+      <c r="H20" s="9">
         <v>15848</v>
       </c>
-      <c r="H20" s="9">
+      <c r="I20" s="9">
         <v>18</v>
       </c>
-      <c r="I20" s="11">
+      <c r="J20" s="11">
         <v>59.2</v>
       </c>
-      <c r="J20" s="11"/>
-      <c r="K20" s="9"/>
+      <c r="K20" s="11"/>
       <c r="L20" s="9"/>
-      <c r="M20" s="11"/>
+      <c r="M20" s="9"/>
       <c r="N20" s="11"/>
-      <c r="O20" s="9"/>
+      <c r="O20" s="11"/>
       <c r="P20" s="9"/>
-      <c r="Q20" s="11"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q20" s="9"/>
+      <c r="R20" s="11"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="11"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="10"/>
       <c r="F21" s="11"/>
-      <c r="G21" s="9">
+      <c r="G21" s="11"/>
+      <c r="H21" s="9">
         <v>13180</v>
       </c>
-      <c r="H21" s="9">
+      <c r="I21" s="9">
         <v>15</v>
       </c>
-      <c r="I21" s="11">
+      <c r="J21" s="11">
         <v>44.9</v>
       </c>
-      <c r="J21" s="11"/>
-      <c r="K21" s="9"/>
+      <c r="K21" s="11"/>
       <c r="L21" s="9"/>
-      <c r="M21" s="11"/>
+      <c r="M21" s="9"/>
       <c r="N21" s="11"/>
-      <c r="O21" s="9"/>
+      <c r="O21" s="11"/>
       <c r="P21" s="9"/>
-      <c r="Q21" s="11"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q21" s="9"/>
+      <c r="R21" s="11"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="9">
+      <c r="G22" s="11"/>
+      <c r="H22" s="9">
         <v>10581</v>
       </c>
-      <c r="H22" s="9">
+      <c r="I22" s="9">
         <v>12</v>
       </c>
-      <c r="I22" s="11">
+      <c r="J22" s="11">
         <v>38.299999999999997</v>
       </c>
-      <c r="J22" s="11"/>
-      <c r="K22" s="9"/>
+      <c r="K22" s="11"/>
       <c r="L22" s="9"/>
-      <c r="M22" s="11"/>
+      <c r="M22" s="9"/>
       <c r="N22" s="11"/>
-      <c r="O22" s="9">
+      <c r="O22" s="11"/>
+      <c r="P22" s="9">
         <v>14278</v>
       </c>
-      <c r="P22" s="9">
+      <c r="Q22" s="9">
         <v>12</v>
       </c>
-      <c r="Q22" s="11">
+      <c r="R22" s="11">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10"/>
       <c r="F23" s="11"/>
-      <c r="G23" s="9">
+      <c r="G23" s="11"/>
+      <c r="H23" s="9">
         <v>6950</v>
       </c>
-      <c r="H23" s="9">
+      <c r="I23" s="9">
         <v>8</v>
       </c>
-      <c r="I23" s="11">
+      <c r="J23" s="11">
         <v>31.7</v>
       </c>
-      <c r="J23" s="11"/>
-      <c r="K23" s="9"/>
+      <c r="K23" s="11"/>
       <c r="L23" s="9"/>
-      <c r="M23" s="11"/>
+      <c r="M23" s="9"/>
       <c r="N23" s="11"/>
-      <c r="O23" s="9">
+      <c r="O23" s="11"/>
+      <c r="P23" s="9">
         <v>10682</v>
       </c>
-      <c r="P23" s="9">
+      <c r="Q23" s="9">
         <v>9</v>
       </c>
-      <c r="Q23" s="11">
+      <c r="R23" s="11">
         <v>38.799999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="11"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="10"/>
       <c r="F24" s="11"/>
-      <c r="G24" s="9">
+      <c r="G24" s="11"/>
+      <c r="H24" s="9">
         <v>3560</v>
       </c>
-      <c r="H24" s="9">
+      <c r="I24" s="9">
         <v>4</v>
       </c>
-      <c r="I24" s="11">
+      <c r="J24" s="11">
         <v>25.9</v>
       </c>
-      <c r="J24" s="11"/>
-      <c r="K24" s="9">
+      <c r="K24" s="11"/>
+      <c r="L24" s="9">
         <v>4097</v>
       </c>
-      <c r="L24" s="9">
+      <c r="M24" s="9">
         <v>4</v>
       </c>
-      <c r="M24" s="11">
+      <c r="N24" s="11">
         <v>25.2</v>
       </c>
-      <c r="N24" s="11"/>
-      <c r="O24" s="9">
+      <c r="O24" s="11"/>
+      <c r="P24" s="9">
         <v>5651</v>
       </c>
-      <c r="P24" s="9">
+      <c r="Q24" s="9">
         <v>5</v>
       </c>
-      <c r="Q24" s="11">
+      <c r="R24" s="11">
         <v>27.2</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="8"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="11"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="10"/>
       <c r="F25" s="11"/>
-      <c r="G25" s="9">
+      <c r="G25" s="11"/>
+      <c r="H25" s="9">
         <v>1951</v>
       </c>
-      <c r="H25" s="9">
+      <c r="I25" s="9">
         <v>2</v>
       </c>
-      <c r="I25" s="11">
+      <c r="J25" s="11">
         <v>15.4</v>
       </c>
-      <c r="J25" s="11"/>
-      <c r="K25" s="9">
+      <c r="K25" s="11"/>
+      <c r="L25" s="9">
         <v>2008</v>
       </c>
-      <c r="L25" s="9">
+      <c r="M25" s="9">
         <v>2</v>
       </c>
-      <c r="M25" s="11">
+      <c r="N25" s="11">
         <v>14.5</v>
       </c>
-      <c r="N25" s="11"/>
-      <c r="O25" s="9">
+      <c r="O25" s="11"/>
+      <c r="P25" s="9">
         <v>2289</v>
       </c>
-      <c r="P25" s="9">
+      <c r="Q25" s="9">
         <v>2</v>
       </c>
-      <c r="Q25" s="11">
+      <c r="R25" s="11">
         <v>14.3</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="7"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="11"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10"/>
       <c r="F26" s="11"/>
-      <c r="G26" s="9"/>
+      <c r="G26" s="11"/>
       <c r="H26" s="9"/>
-      <c r="I26" s="11"/>
+      <c r="I26" s="9"/>
       <c r="J26" s="11"/>
-      <c r="K26" s="9"/>
+      <c r="K26" s="11"/>
       <c r="L26" s="9"/>
-      <c r="M26" s="11"/>
+      <c r="M26" s="9"/>
       <c r="N26" s="11"/>
-      <c r="O26" s="9"/>
+      <c r="O26" s="11"/>
       <c r="P26" s="9"/>
-      <c r="Q26" s="11"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q26" s="9"/>
+      <c r="R26" s="11"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="11"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="10"/>
       <c r="F27" s="11"/>
-      <c r="G27" s="9">
+      <c r="G27" s="11"/>
+      <c r="H27" s="9">
         <v>21945</v>
       </c>
-      <c r="H27" s="9">
+      <c r="I27" s="9">
         <v>24</v>
       </c>
-      <c r="I27" s="11">
+      <c r="J27" s="11">
         <v>62.2</v>
       </c>
-      <c r="J27" s="11"/>
-      <c r="K27" s="9">
+      <c r="K27" s="11"/>
+      <c r="L27" s="9">
         <v>25200</v>
       </c>
-      <c r="L27" s="9">
+      <c r="M27" s="9">
         <v>25</v>
       </c>
-      <c r="M27" s="11">
+      <c r="N27" s="11">
         <v>68.2</v>
       </c>
-      <c r="N27" s="11"/>
-      <c r="O27" s="9">
+      <c r="O27" s="11"/>
+      <c r="P27" s="9">
         <v>27683</v>
       </c>
-      <c r="P27" s="9">
+      <c r="Q27" s="9">
         <v>24</v>
       </c>
-      <c r="Q27" s="11">
+      <c r="R27" s="11">
         <v>72.599999999999994</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="11"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="10"/>
       <c r="F28" s="11"/>
-      <c r="G28" s="9">
+      <c r="G28" s="11"/>
+      <c r="H28" s="9">
         <v>12461</v>
       </c>
-      <c r="H28" s="9">
+      <c r="I28" s="9">
         <v>14</v>
       </c>
-      <c r="I28" s="11">
+      <c r="J28" s="11">
         <v>25.8</v>
       </c>
-      <c r="J28" s="11"/>
-      <c r="K28" s="9">
+      <c r="K28" s="11"/>
+      <c r="L28" s="9">
         <v>14581</v>
       </c>
-      <c r="L28" s="9">
+      <c r="M28" s="9">
         <v>14</v>
       </c>
-      <c r="M28" s="11">
+      <c r="N28" s="11">
         <v>26.4</v>
       </c>
-      <c r="N28" s="11"/>
-      <c r="O28" s="9">
+      <c r="O28" s="11"/>
+      <c r="P28" s="9">
         <v>18625</v>
       </c>
-      <c r="P28" s="9">
+      <c r="Q28" s="9">
         <v>16</v>
       </c>
-      <c r="Q28" s="11">
+      <c r="R28" s="11">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="7"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C29" s="7"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B30" s="8"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="11"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="10"/>
       <c r="F30" s="11"/>
-      <c r="G30" s="9">
+      <c r="G30" s="11"/>
+      <c r="H30" s="9">
         <v>51159</v>
       </c>
-      <c r="H30" s="9">
+      <c r="I30" s="9">
         <v>57</v>
       </c>
-      <c r="I30" s="11">
+      <c r="J30" s="11">
         <v>52.2</v>
       </c>
-      <c r="J30" s="11"/>
-      <c r="K30" s="9">
+      <c r="K30" s="11"/>
+      <c r="L30" s="9">
         <v>57689</v>
       </c>
-      <c r="L30" s="9">
+      <c r="M30" s="9">
         <v>56</v>
       </c>
-      <c r="M30" s="11">
+      <c r="N30" s="11">
         <v>54.3</v>
       </c>
-      <c r="N30" s="11"/>
-      <c r="O30" s="9">
+      <c r="O30" s="11"/>
+      <c r="P30" s="9">
         <v>67407</v>
       </c>
-      <c r="P30" s="9">
+      <c r="Q30" s="9">
         <v>58</v>
       </c>
-      <c r="Q30" s="11">
+      <c r="R30" s="11">
         <v>58.4</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B31" s="8"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="11"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="10"/>
       <c r="F31" s="11"/>
-      <c r="G31" s="9">
+      <c r="G31" s="11"/>
+      <c r="H31" s="9">
         <v>38569</v>
       </c>
-      <c r="H31" s="9">
+      <c r="I31" s="9">
         <v>43</v>
       </c>
-      <c r="I31" s="11">
+      <c r="J31" s="11">
         <v>38.4</v>
       </c>
-      <c r="J31" s="11"/>
-      <c r="K31" s="9">
+      <c r="K31" s="11"/>
+      <c r="L31" s="9">
         <v>44746</v>
       </c>
-      <c r="L31" s="9">
+      <c r="M31" s="9">
         <v>44</v>
       </c>
-      <c r="M31" s="11">
+      <c r="N31" s="11">
         <v>41.2</v>
       </c>
-      <c r="N31" s="11"/>
-      <c r="O31" s="9">
+      <c r="O31" s="11"/>
+      <c r="P31" s="9">
         <v>49017</v>
       </c>
-      <c r="P31" s="9">
+      <c r="Q31" s="9">
         <v>42</v>
       </c>
-      <c r="Q31" s="11">
+      <c r="R31" s="11">
         <v>41.3</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B32" s="7"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B33" s="8"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="11"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="10"/>
       <c r="F33" s="11"/>
-      <c r="G33" s="9">
+      <c r="G33" s="11"/>
+      <c r="H33" s="9">
         <v>25950</v>
       </c>
-      <c r="H33" s="9">
+      <c r="I33" s="9">
         <v>29</v>
       </c>
-      <c r="I33" s="11">
+      <c r="J33" s="11">
         <v>570.6</v>
       </c>
-      <c r="J33" s="11"/>
-      <c r="K33" s="9">
+      <c r="K33" s="11"/>
+      <c r="L33" s="9">
         <v>26718</v>
       </c>
-      <c r="L33" s="9">
+      <c r="M33" s="9">
         <v>26</v>
       </c>
-      <c r="M33" s="11">
+      <c r="N33" s="11">
         <v>487.4</v>
       </c>
-      <c r="N33" s="11"/>
-      <c r="O33" s="9">
+      <c r="O33" s="11"/>
+      <c r="P33" s="9">
         <v>23437</v>
       </c>
-      <c r="P33" s="9">
+      <c r="Q33" s="9">
         <v>20</v>
       </c>
-      <c r="Q33" s="11">
+      <c r="R33" s="11">
         <v>361</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B34" s="8"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="11"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="10"/>
       <c r="F34" s="11"/>
-      <c r="G34" s="9">
+      <c r="G34" s="11"/>
+      <c r="H34" s="9">
         <v>57324</v>
       </c>
-      <c r="H34" s="9">
+      <c r="I34" s="9">
         <v>64</v>
       </c>
-      <c r="I34" s="11">
+      <c r="J34" s="11">
         <v>31.4</v>
       </c>
-      <c r="J34" s="11"/>
-      <c r="K34" s="9">
+      <c r="K34" s="11"/>
+      <c r="L34" s="9">
         <v>68070</v>
       </c>
-      <c r="L34" s="9">
+      <c r="M34" s="9">
         <v>66</v>
       </c>
-      <c r="M34" s="11">
+      <c r="N34" s="11">
         <v>34.200000000000003</v>
       </c>
-      <c r="N34" s="11"/>
-      <c r="O34" s="9">
+      <c r="O34" s="11"/>
+      <c r="P34" s="9">
         <v>80769</v>
       </c>
-      <c r="P34" s="9">
+      <c r="Q34" s="9">
         <v>69</v>
       </c>
-      <c r="Q34" s="11">
+      <c r="R34" s="11">
         <v>37.799999999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="8"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="11"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="10"/>
       <c r="F35" s="11"/>
-      <c r="G35" s="9">
+      <c r="G35" s="11"/>
+      <c r="H35" s="9">
         <v>6454</v>
       </c>
-      <c r="H35" s="9">
+      <c r="I35" s="9">
         <v>7</v>
       </c>
-      <c r="I35" s="11">
+      <c r="J35" s="11">
         <v>57</v>
       </c>
-      <c r="J35" s="11"/>
-      <c r="K35" s="9">
+      <c r="K35" s="11"/>
+      <c r="L35" s="9">
         <v>7651</v>
       </c>
-      <c r="L35" s="9">
+      <c r="M35" s="9">
         <v>7</v>
       </c>
-      <c r="M35" s="11">
+      <c r="N35" s="11">
         <v>72.3</v>
       </c>
-      <c r="N35" s="11"/>
-      <c r="O35" s="9">
+      <c r="O35" s="11"/>
+      <c r="P35" s="9">
         <v>12217</v>
       </c>
-      <c r="P35" s="9">
+      <c r="Q35" s="9">
         <v>10</v>
       </c>
-      <c r="Q35" s="11">
+      <c r="R35" s="11">
         <v>86.6</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="7"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C36" s="7"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>37</v>
       </c>
       <c r="B37" s="8"/>
-      <c r="C37" s="9">
+      <c r="C37" s="8"/>
+      <c r="D37" s="9">
         <v>23041</v>
       </c>
-      <c r="D37" s="10">
+      <c r="E37" s="10">
         <v>24</v>
       </c>
-      <c r="E37" s="11">
+      <c r="F37" s="11">
         <v>36.4</v>
       </c>
-      <c r="F37" s="11"/>
-      <c r="G37" s="9"/>
+      <c r="G37" s="11"/>
       <c r="H37" s="9"/>
-      <c r="I37" s="11"/>
+      <c r="I37" s="9"/>
       <c r="J37" s="11"/>
-      <c r="K37" s="9">
+      <c r="K37" s="11"/>
+      <c r="L37" s="9">
         <v>27479</v>
       </c>
-      <c r="L37" s="9">
+      <c r="M37" s="9">
         <v>27</v>
       </c>
-      <c r="M37" s="11">
+      <c r="N37" s="11">
         <v>39.700000000000003</v>
       </c>
-      <c r="N37" s="11"/>
-      <c r="O37" s="9">
+      <c r="O37" s="11"/>
+      <c r="P37" s="9">
         <v>37715</v>
       </c>
-      <c r="P37" s="9">
+      <c r="Q37" s="9">
         <v>32</v>
       </c>
-      <c r="Q37" s="11">
+      <c r="R37" s="11">
         <v>50.4</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="8"/>
-      <c r="C38" s="9">
+      <c r="C38" s="8"/>
+      <c r="D38" s="9">
         <v>18154</v>
       </c>
-      <c r="D38" s="10">
+      <c r="E38" s="10">
         <v>19</v>
       </c>
-      <c r="E38" s="11">
+      <c r="F38" s="11">
         <v>38.9</v>
       </c>
-      <c r="F38" s="11"/>
-      <c r="G38" s="9"/>
+      <c r="G38" s="11"/>
       <c r="H38" s="9"/>
-      <c r="I38" s="11"/>
+      <c r="I38" s="9"/>
       <c r="J38" s="11"/>
-      <c r="K38" s="9">
+      <c r="K38" s="11"/>
+      <c r="L38" s="9">
         <v>22306</v>
       </c>
-      <c r="L38" s="9">
+      <c r="M38" s="9">
         <v>22</v>
       </c>
-      <c r="M38" s="11">
+      <c r="N38" s="11">
         <v>41.7</v>
       </c>
-      <c r="N38" s="11"/>
-      <c r="O38" s="9"/>
+      <c r="O38" s="11"/>
       <c r="P38" s="9"/>
-      <c r="Q38" s="11"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q38" s="9"/>
+      <c r="R38" s="11"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B39" s="8"/>
-      <c r="C39" s="9">
+      <c r="C39" s="8"/>
+      <c r="D39" s="9">
         <v>19316</v>
       </c>
-      <c r="D39" s="10">
+      <c r="E39" s="10">
         <v>20</v>
       </c>
-      <c r="E39" s="11">
+      <c r="F39" s="11">
         <v>54.8</v>
       </c>
-      <c r="F39" s="11"/>
-      <c r="G39" s="9"/>
+      <c r="G39" s="11"/>
       <c r="H39" s="9"/>
-      <c r="I39" s="11"/>
+      <c r="I39" s="9"/>
       <c r="J39" s="11"/>
-      <c r="K39" s="9">
+      <c r="K39" s="11"/>
+      <c r="L39" s="9">
         <v>19039</v>
       </c>
-      <c r="L39" s="9">
+      <c r="M39" s="9">
         <v>19</v>
       </c>
-      <c r="M39" s="11">
+      <c r="N39" s="11">
         <v>43.9</v>
       </c>
-      <c r="N39" s="11"/>
-      <c r="O39" s="9"/>
+      <c r="O39" s="11"/>
       <c r="P39" s="9"/>
-      <c r="Q39" s="11"/>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q39" s="9"/>
+      <c r="R39" s="11"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B40" s="8"/>
-      <c r="C40" s="9">
+      <c r="C40" s="8"/>
+      <c r="D40" s="9">
         <v>5844</v>
       </c>
-      <c r="D40" s="10">
+      <c r="E40" s="10">
         <v>6</v>
       </c>
-      <c r="E40" s="11">
+      <c r="F40" s="11">
         <v>39.799999999999997</v>
       </c>
-      <c r="F40" s="11"/>
-      <c r="G40" s="9"/>
+      <c r="G40" s="11"/>
       <c r="H40" s="9"/>
-      <c r="I40" s="11"/>
+      <c r="I40" s="9"/>
       <c r="J40" s="11"/>
-      <c r="K40" s="9">
+      <c r="K40" s="11"/>
+      <c r="L40" s="9">
         <v>5816</v>
       </c>
-      <c r="L40" s="9">
+      <c r="M40" s="9">
         <v>6</v>
       </c>
-      <c r="M40" s="11">
+      <c r="N40" s="11">
         <v>36.4</v>
       </c>
-      <c r="N40" s="11"/>
-      <c r="O40" s="9"/>
+      <c r="O40" s="11"/>
       <c r="P40" s="9"/>
-      <c r="Q40" s="11"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q40" s="9"/>
+      <c r="R40" s="11"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B41" s="8"/>
-      <c r="C41" s="9">
+      <c r="C41" s="8"/>
+      <c r="D41" s="9">
         <v>9799</v>
       </c>
-      <c r="D41" s="10">
+      <c r="E41" s="10">
         <v>10</v>
       </c>
-      <c r="E41" s="11">
+      <c r="F41" s="11">
         <v>53.6</v>
       </c>
-      <c r="F41" s="11"/>
-      <c r="G41" s="9">
+      <c r="G41" s="11"/>
+      <c r="H41" s="9">
         <v>8277</v>
       </c>
-      <c r="H41" s="9">
+      <c r="I41" s="9">
         <v>9</v>
       </c>
-      <c r="I41" s="11">
+      <c r="J41" s="11">
         <v>42.3</v>
       </c>
-      <c r="J41" s="11"/>
-      <c r="K41" s="9">
+      <c r="K41" s="11"/>
+      <c r="L41" s="9">
         <v>9191</v>
       </c>
-      <c r="L41" s="9">
+      <c r="M41" s="9">
         <v>9</v>
       </c>
-      <c r="M41" s="11">
+      <c r="N41" s="11">
         <v>41</v>
       </c>
-      <c r="N41" s="11"/>
-      <c r="O41" s="9"/>
+      <c r="O41" s="11"/>
       <c r="P41" s="9"/>
-      <c r="Q41" s="11"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q41" s="9"/>
+      <c r="R41" s="11"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B42" s="8"/>
-      <c r="C42" s="9">
+      <c r="C42" s="8"/>
+      <c r="D42" s="9">
         <v>1264</v>
       </c>
-      <c r="D42" s="10">
+      <c r="E42" s="10">
         <v>1</v>
       </c>
-      <c r="E42" s="11">
+      <c r="F42" s="11">
         <v>27.5</v>
       </c>
-      <c r="F42" s="11"/>
-      <c r="G42" s="9">
+      <c r="G42" s="11"/>
+      <c r="H42" s="9">
         <v>1145</v>
       </c>
-      <c r="H42" s="9">
+      <c r="I42" s="9">
         <v>1</v>
       </c>
-      <c r="I42" s="11">
+      <c r="J42" s="11">
         <v>24</v>
       </c>
-      <c r="J42" s="11"/>
-      <c r="K42" s="9">
+      <c r="K42" s="11"/>
+      <c r="L42" s="9">
         <v>1537</v>
       </c>
-      <c r="L42" s="9">
+      <c r="M42" s="9">
         <v>2</v>
       </c>
-      <c r="M42" s="11">
+      <c r="N42" s="11">
         <v>31</v>
       </c>
-      <c r="N42" s="11"/>
-      <c r="O42" s="9">
+      <c r="O42" s="11"/>
+      <c r="P42" s="9">
         <v>1622</v>
       </c>
-      <c r="P42" s="9">
+      <c r="Q42" s="9">
         <v>1</v>
       </c>
-      <c r="Q42" s="11">
+      <c r="R42" s="11">
         <v>31.8</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B43" s="8"/>
-      <c r="C43" s="9">
+      <c r="C43" s="8"/>
+      <c r="D43" s="9">
         <v>16948</v>
       </c>
-      <c r="D43" s="10">
+      <c r="E43" s="10">
         <v>18</v>
       </c>
-      <c r="E43" s="11">
+      <c r="F43" s="11">
         <v>904.4</v>
       </c>
-      <c r="F43" s="11"/>
-      <c r="G43" s="9">
+      <c r="G43" s="11"/>
+      <c r="H43" s="9">
         <v>15265</v>
       </c>
-      <c r="H43" s="9">
+      <c r="I43" s="9">
         <v>17</v>
       </c>
-      <c r="I43" s="11">
+      <c r="J43" s="11">
         <v>791.7</v>
       </c>
-      <c r="J43" s="11"/>
-      <c r="K43" s="9">
+      <c r="K43" s="11"/>
+      <c r="L43" s="9">
         <v>15330</v>
       </c>
-      <c r="L43" s="9">
+      <c r="M43" s="9">
         <v>15</v>
       </c>
-      <c r="M43" s="11">
+      <c r="N43" s="11">
         <v>723.3</v>
       </c>
-      <c r="N43" s="11"/>
-      <c r="O43" s="9">
+      <c r="O43" s="11"/>
+      <c r="P43" s="9">
         <v>13717</v>
       </c>
-      <c r="P43" s="9">
+      <c r="Q43" s="9">
         <v>12</v>
       </c>
-      <c r="Q43" s="11">
+      <c r="R43" s="11">
         <v>599.4</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B44" s="8"/>
-      <c r="C44" s="9">
+      <c r="C44" s="8"/>
+      <c r="D44" s="9">
         <v>943</v>
       </c>
-      <c r="D44" s="10">
+      <c r="E44" s="10">
         <v>1</v>
       </c>
-      <c r="E44" s="11">
+      <c r="F44" s="11">
         <v>30.4</v>
       </c>
-      <c r="F44" s="11"/>
-      <c r="G44" s="9">
+      <c r="G44" s="11"/>
+      <c r="H44" s="9">
         <v>949</v>
       </c>
-      <c r="H44" s="9">
+      <c r="I44" s="9">
         <v>1</v>
       </c>
-      <c r="I44" s="11">
+      <c r="J44" s="11">
         <v>29.3</v>
       </c>
-      <c r="J44" s="11"/>
-      <c r="K44" s="9">
+      <c r="K44" s="11"/>
+      <c r="L44" s="9">
         <v>1738</v>
       </c>
-      <c r="L44" s="9">
+      <c r="M44" s="9">
         <v>2</v>
       </c>
-      <c r="M44" s="11">
+      <c r="N44" s="11">
         <v>48.7</v>
       </c>
-      <c r="N44" s="11"/>
-      <c r="O44" s="9">
+      <c r="O44" s="11"/>
+      <c r="P44" s="9">
         <v>1596</v>
       </c>
-      <c r="P44" s="9">
+      <c r="Q44" s="9">
         <v>1</v>
       </c>
-      <c r="Q44" s="11">
+      <c r="R44" s="11">
         <v>40.200000000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B45" s="16"/>
-      <c r="C45" s="17">
+      <c r="C45" s="16"/>
+      <c r="D45" s="17">
         <v>95314</v>
       </c>
-      <c r="D45" s="18">
+      <c r="E45" s="18">
         <v>100</v>
       </c>
-      <c r="E45" s="19">
+      <c r="F45" s="19">
         <v>50.8</v>
       </c>
-      <c r="F45" s="19"/>
-      <c r="G45" s="17">
+      <c r="G45" s="19"/>
+      <c r="H45" s="17">
         <v>89728</v>
       </c>
-      <c r="H45" s="17">
+      <c r="I45" s="17">
         <v>100</v>
       </c>
-      <c r="I45" s="19">
+      <c r="J45" s="19">
         <v>45.2</v>
       </c>
-      <c r="J45" s="19"/>
-      <c r="K45" s="17">
+      <c r="K45" s="19"/>
+      <c r="L45" s="17">
         <v>102439</v>
       </c>
-      <c r="L45" s="17">
+      <c r="M45" s="17">
         <v>100</v>
       </c>
-      <c r="M45" s="19">
+      <c r="N45" s="19">
         <v>47.6</v>
       </c>
-      <c r="N45" s="19"/>
-      <c r="O45" s="17">
+      <c r="O45" s="19"/>
+      <c r="P45" s="17">
         <v>116427</v>
       </c>
-      <c r="P45" s="17">
+      <c r="Q45" s="17">
         <v>100</v>
       </c>
-      <c r="Q45" s="19">
+      <c r="R45" s="19">
         <v>49.8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A7:Q7"/>
-    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A7:R7"/>
+    <mergeCell ref="A1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>